<commit_message>
Fixed the information matrix
See above
</commit_message>
<xml_diff>
--- a/DataMatrixInformation.xlsx
+++ b/DataMatrixInformation.xlsx
@@ -1,15 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="27510"/>
+  <workbookPr filterPrivacy="1"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Mason/Dropbox/ECE 4335/Repository/Senior Design/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="14500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -236,7 +249,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -255,6 +268,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -280,7 +299,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -300,11 +319,38 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -363,9 +409,9 @@
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -398,9 +444,9 @@
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -604,19 +650,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BK11"/>
+  <dimension ref="A1:BK28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BB1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="BK5" sqref="BK5"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.7109375" defaultRowHeight="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.6640625" defaultRowHeight="17" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="17.7109375" style="1"/>
+    <col min="1" max="1" width="20.6640625" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="17.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:63" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:63" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>71</v>
       </c>
@@ -719,7 +765,7 @@
       <c r="AH1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AI1" s="7" t="s">
         <v>3</v>
       </c>
       <c r="AJ1" s="1" t="s">
@@ -755,7 +801,7 @@
       <c r="AT1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="AU1" s="1" t="s">
+      <c r="AU1" s="8" t="s">
         <v>42</v>
       </c>
       <c r="AV1" s="1" t="s">
@@ -807,7 +853,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:63" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:63" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>60</v>
       </c>
@@ -998,7 +1044,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:63" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:63" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>61</v>
       </c>
@@ -1102,7 +1148,7 @@
         <v>0</v>
       </c>
       <c r="AI3" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ3" s="1">
         <v>0</v>
@@ -1189,7 +1235,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:63" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:63" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>62</v>
       </c>
@@ -1380,7 +1426,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:63" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:63" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>63</v>
       </c>
@@ -1484,7 +1530,7 @@
         <v>0</v>
       </c>
       <c r="AI5" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ5" s="1">
         <v>0</v>
@@ -1571,7 +1617,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:63" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:63" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>64</v>
       </c>
@@ -1711,7 +1757,7 @@
         <v>1</v>
       </c>
       <c r="AU6" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AV6" s="1">
         <v>0</v>
@@ -1762,7 +1808,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:63" s="4" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:63" s="4" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>65</v>
       </c>
@@ -1865,7 +1911,7 @@
       <c r="AH7" s="5">
         <v>0</v>
       </c>
-      <c r="AI7" s="5">
+      <c r="AI7" s="1">
         <v>0</v>
       </c>
       <c r="AJ7" s="5">
@@ -1901,7 +1947,7 @@
       <c r="AT7" s="5">
         <v>0</v>
       </c>
-      <c r="AU7" s="5">
+      <c r="AU7" s="1">
         <v>0</v>
       </c>
       <c r="AV7" s="5">
@@ -1953,7 +1999,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:63" s="4" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:63" s="4" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>66</v>
       </c>
@@ -2056,7 +2102,7 @@
       <c r="AH8" s="5">
         <v>0</v>
       </c>
-      <c r="AI8" s="5">
+      <c r="AI8" s="1">
         <v>0</v>
       </c>
       <c r="AJ8" s="5">
@@ -2092,7 +2138,7 @@
       <c r="AT8" s="5">
         <v>0</v>
       </c>
-      <c r="AU8" s="5">
+      <c r="AU8" s="1">
         <v>0</v>
       </c>
       <c r="AV8" s="5">
@@ -2144,7 +2190,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:63" s="4" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:63" s="4" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>67</v>
       </c>
@@ -2161,7 +2207,7 @@
         <v>1</v>
       </c>
       <c r="F9" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G9" s="6">
         <v>1</v>
@@ -2247,8 +2293,8 @@
       <c r="AH9" s="5">
         <v>0</v>
       </c>
-      <c r="AI9" s="5">
-        <v>0</v>
+      <c r="AI9" s="1">
+        <v>1</v>
       </c>
       <c r="AJ9" s="5">
         <v>0</v>
@@ -2283,7 +2329,7 @@
       <c r="AT9" s="5">
         <v>0</v>
       </c>
-      <c r="AU9" s="5">
+      <c r="AU9" s="1">
         <v>0</v>
       </c>
       <c r="AV9" s="5">
@@ -2335,7 +2381,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:63" s="4" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:63" s="4" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>68</v>
       </c>
@@ -2438,8 +2484,8 @@
       <c r="AH10" s="5">
         <v>0</v>
       </c>
-      <c r="AI10" s="5">
-        <v>0</v>
+      <c r="AI10" s="1">
+        <v>1</v>
       </c>
       <c r="AJ10" s="5">
         <v>0</v>
@@ -2474,7 +2520,7 @@
       <c r="AT10" s="5">
         <v>0</v>
       </c>
-      <c r="AU10" s="5">
+      <c r="AU10" s="1">
         <v>0</v>
       </c>
       <c r="AV10" s="5">
@@ -2526,7 +2572,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:63" s="4" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:63" s="4" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>69</v>
       </c>
@@ -2629,7 +2675,7 @@
       <c r="AH11" s="6">
         <v>1</v>
       </c>
-      <c r="AI11" s="5">
+      <c r="AI11" s="1">
         <v>0</v>
       </c>
       <c r="AJ11" s="5">
@@ -2665,7 +2711,7 @@
       <c r="AT11" s="5">
         <v>0</v>
       </c>
-      <c r="AU11" s="5">
+      <c r="AU11" s="1">
         <v>0</v>
       </c>
       <c r="AV11" s="5">
@@ -2716,8 +2762,293 @@
       <c r="BK11" s="5">
         <v>0</v>
       </c>
+    </row>
+    <row r="13" spans="1:63" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B13" s="1">
+        <f>SUM(B2:B11)</f>
+        <v>3</v>
+      </c>
+      <c r="C13" s="1">
+        <f t="shared" ref="C13:BK13" si="0">SUM(C2:C11)</f>
+        <v>2</v>
+      </c>
+      <c r="D13" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E13" s="1">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="F13" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G13" s="1">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="H13" s="1">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="I13" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="J13" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K13" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="L13" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="M13" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="N13" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="O13" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="P13" s="1">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="Q13" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="R13" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="S13" s="1">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="T13" s="1">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="U13" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="V13" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="W13" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="X13" s="1">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="Y13" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="Z13" s="1">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="AA13" s="1">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="AB13" s="1">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="AC13" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="AD13" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="AE13" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="AF13" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="AG13" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="AH13" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="AI13" s="1">
+        <f>SUM(AI2:AI11)</f>
+        <v>4</v>
+      </c>
+      <c r="AJ13" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="AK13" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="AL13" s="1">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="AM13" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="AN13" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="AO13" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="AP13" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="AQ13" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="AR13" s="1">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="AS13" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="AT13" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="AU13" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="AV13" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="AW13" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="AX13" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="AY13" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="AZ13" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="BA13" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="BB13" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="BC13" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="BD13" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="BE13" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="BF13" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="BG13" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="BH13" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="BI13" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="BJ13" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="BK13" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="2"/>
+    </row>
+    <row r="20" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="2"/>
+    </row>
+    <row r="21" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="2"/>
+    </row>
+    <row r="22" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="2"/>
+    </row>
+    <row r="23" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="2"/>
+    </row>
+    <row r="24" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="3"/>
+    </row>
+    <row r="25" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="3"/>
+    </row>
+    <row r="26" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="3"/>
+    </row>
+    <row r="27" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="3"/>
+    </row>
+    <row r="28" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="3"/>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="B13:BK13">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
This is what i've done so far
I summed up the number of times each symptom occurred, and used that to
order them from most to least significant when creating the new
multiplier
</commit_message>
<xml_diff>
--- a/DataMatrixInformation.xlsx
+++ b/DataMatrixInformation.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="72">
   <si>
     <t>Body Ache</t>
   </si>
@@ -249,7 +249,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -278,6 +278,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -296,8 +312,68 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -326,20 +402,70 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="61">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -652,8 +778,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BK28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" zoomScale="117" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="BK20" sqref="BK20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.6640625" defaultRowHeight="17" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -667,190 +793,190 @@
         <v>71</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AA1" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AO1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="AP1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AQ1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="AR1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="AS1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AT1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AU1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AV1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AW1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AX1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AY1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="AZ1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="BA1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="BB1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="BC1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="BD1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="BE1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="BF1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="BG1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="BH1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="BI1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="BJ1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="BK1" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AD1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="AE1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="AF1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="AG1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="AH1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AI1" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="AJ1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="AK1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="AL1" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="AM1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="AN1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="AO1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="AP1" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="AQ1" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="AR1" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="AS1" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="AT1" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="AU1" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="AV1" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="AW1" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="AX1" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="AY1" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="AZ1" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="BA1" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="BB1" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="BC1" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="BD1" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="BE1" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="BF1" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="BG1" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="BH1" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="BI1" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="BJ1" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="BK1" s="1" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:63" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -870,10 +996,10 @@
         <v>0</v>
       </c>
       <c r="F2" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H2" s="1">
         <v>0</v>
@@ -885,10 +1011,10 @@
         <v>0</v>
       </c>
       <c r="K2" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M2" s="1">
         <v>0</v>
@@ -909,13 +1035,13 @@
         <v>0</v>
       </c>
       <c r="S2" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T2" s="1">
         <v>0</v>
       </c>
       <c r="U2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V2" s="1">
         <v>0</v>
@@ -954,22 +1080,22 @@
         <v>0</v>
       </c>
       <c r="AH2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI2" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK2" s="1">
         <v>0</v>
       </c>
       <c r="AL2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AM2" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN2" s="1">
         <v>0</v>
@@ -987,7 +1113,7 @@
         <v>0</v>
       </c>
       <c r="AS2" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AT2" s="1">
         <v>0</v>
@@ -1020,7 +1146,7 @@
         <v>0</v>
       </c>
       <c r="BD2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BE2" s="1">
         <v>0</v>
@@ -1035,7 +1161,7 @@
         <v>0</v>
       </c>
       <c r="BI2" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BJ2" s="1">
         <v>1</v>
@@ -1058,7 +1184,7 @@
         <v>0</v>
       </c>
       <c r="E3" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F3" s="1">
         <v>0</v>
@@ -1115,7 +1241,7 @@
         <v>0</v>
       </c>
       <c r="X3" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y3" s="1">
         <v>0</v>
@@ -1148,10 +1274,10 @@
         <v>0</v>
       </c>
       <c r="AI3" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ3" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK3" s="1">
         <v>0</v>
@@ -1184,7 +1310,7 @@
         <v>0</v>
       </c>
       <c r="AU3" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AV3" s="1">
         <v>0</v>
@@ -1214,13 +1340,13 @@
         <v>0</v>
       </c>
       <c r="BE3" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BF3" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BG3" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BH3" s="1">
         <v>0</v>
@@ -1279,13 +1405,13 @@
         <v>0</v>
       </c>
       <c r="O4" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P4" s="1">
         <v>0</v>
       </c>
       <c r="Q4" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R4" s="1">
         <v>0</v>
@@ -1294,7 +1420,7 @@
         <v>0</v>
       </c>
       <c r="T4" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U4" s="1">
         <v>0</v>
@@ -1318,19 +1444,19 @@
         <v>0</v>
       </c>
       <c r="AB4" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC4" s="1">
         <v>0</v>
       </c>
       <c r="AD4" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE4" s="1">
         <v>0</v>
       </c>
       <c r="AF4" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG4" s="1">
         <v>0</v>
@@ -1345,7 +1471,7 @@
         <v>0</v>
       </c>
       <c r="AK4" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AL4" s="1">
         <v>0</v>
@@ -1378,7 +1504,7 @@
         <v>0</v>
       </c>
       <c r="AV4" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AW4" s="1">
         <v>0</v>
@@ -1431,16 +1557,16 @@
         <v>63</v>
       </c>
       <c r="B5" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C5" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D5" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E5" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F5" s="1">
         <v>0</v>
@@ -1449,13 +1575,13 @@
         <v>1</v>
       </c>
       <c r="H5" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I5" s="1">
         <v>0</v>
       </c>
       <c r="J5" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K5" s="1">
         <v>0</v>
@@ -1464,7 +1590,7 @@
         <v>0</v>
       </c>
       <c r="M5" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N5" s="1">
         <v>0</v>
@@ -1476,13 +1602,13 @@
         <v>0</v>
       </c>
       <c r="Q5" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R5" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S5" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T5" s="1">
         <v>0</v>
@@ -1491,19 +1617,19 @@
         <v>0</v>
       </c>
       <c r="V5" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W5" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X5" s="1">
         <v>0</v>
       </c>
       <c r="Y5" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z5" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA5" s="1">
         <v>0</v>
@@ -1512,7 +1638,7 @@
         <v>0</v>
       </c>
       <c r="AC5" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD5" s="1">
         <v>0</v>
@@ -1530,7 +1656,7 @@
         <v>0</v>
       </c>
       <c r="AI5" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ5" s="1">
         <v>0</v>
@@ -1539,7 +1665,7 @@
         <v>0</v>
       </c>
       <c r="AL5" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AM5" s="1">
         <v>0</v>
@@ -1554,40 +1680,40 @@
         <v>1</v>
       </c>
       <c r="AQ5" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AR5" s="1">
         <v>0</v>
       </c>
       <c r="AS5" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AT5" s="1">
         <v>0</v>
       </c>
       <c r="AU5" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AV5" s="1">
         <v>0</v>
       </c>
       <c r="AW5" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AX5" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AY5" s="1">
         <v>0</v>
       </c>
       <c r="AZ5" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BA5" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BB5" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BC5" s="1">
         <v>0</v>
@@ -1599,22 +1725,22 @@
         <v>0</v>
       </c>
       <c r="BF5" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BG5" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BH5" s="1">
         <v>0</v>
       </c>
       <c r="BI5" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BJ5" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BK5" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:63" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -1652,7 +1778,7 @@
         <v>0</v>
       </c>
       <c r="L6" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M6" s="1">
         <v>0</v>
@@ -1664,13 +1790,13 @@
         <v>0</v>
       </c>
       <c r="P6" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q6" s="1">
         <v>0</v>
       </c>
       <c r="R6" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S6" s="1">
         <v>0</v>
@@ -1679,25 +1805,25 @@
         <v>0</v>
       </c>
       <c r="U6" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V6" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W6" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X6" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y6" s="1">
         <v>0</v>
       </c>
       <c r="Z6" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA6" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB6" s="1">
         <v>0</v>
@@ -1709,13 +1835,13 @@
         <v>0</v>
       </c>
       <c r="AE6" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF6" s="1">
         <v>0</v>
       </c>
       <c r="AG6" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH6" s="1">
         <v>0</v>
@@ -1736,7 +1862,7 @@
         <v>0</v>
       </c>
       <c r="AN6" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AO6" s="1">
         <v>0</v>
@@ -1745,19 +1871,19 @@
         <v>0</v>
       </c>
       <c r="AQ6" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AR6" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AS6" s="1">
         <v>0</v>
       </c>
       <c r="AT6" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AU6" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AV6" s="1">
         <v>0</v>
@@ -1812,7 +1938,7 @@
       <c r="A7" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7" s="5">
         <v>0</v>
       </c>
       <c r="C7" s="5">
@@ -1827,8 +1953,8 @@
       <c r="F7" s="5">
         <v>0</v>
       </c>
-      <c r="G7" s="6">
-        <v>1</v>
+      <c r="G7" s="5">
+        <v>0</v>
       </c>
       <c r="H7" s="6">
         <v>1</v>
@@ -1848,14 +1974,14 @@
       <c r="M7" s="5">
         <v>0</v>
       </c>
-      <c r="N7" s="6">
-        <v>1</v>
+      <c r="N7" s="5">
+        <v>0</v>
       </c>
       <c r="O7" s="5">
         <v>0</v>
       </c>
-      <c r="P7" s="6">
-        <v>1</v>
+      <c r="P7" s="5">
+        <v>0</v>
       </c>
       <c r="Q7" s="5">
         <v>0</v>
@@ -1866,8 +1992,8 @@
       <c r="S7" s="5">
         <v>0</v>
       </c>
-      <c r="T7" s="6">
-        <v>1</v>
+      <c r="T7" s="5">
+        <v>0</v>
       </c>
       <c r="U7" s="5">
         <v>0</v>
@@ -1887,11 +2013,11 @@
       <c r="Z7" s="5">
         <v>0</v>
       </c>
-      <c r="AA7" s="5">
-        <v>0</v>
-      </c>
-      <c r="AB7" s="6">
-        <v>1</v>
+      <c r="AA7" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB7" s="5">
+        <v>0</v>
       </c>
       <c r="AC7" s="5">
         <v>0</v>
@@ -1902,23 +2028,23 @@
       <c r="AE7" s="5">
         <v>0</v>
       </c>
-      <c r="AF7" s="5">
-        <v>0</v>
-      </c>
-      <c r="AG7" s="5">
-        <v>0</v>
+      <c r="AF7" s="6">
+        <v>1</v>
+      </c>
+      <c r="AG7" s="6">
+        <v>1</v>
       </c>
       <c r="AH7" s="5">
         <v>0</v>
       </c>
-      <c r="AI7" s="1">
+      <c r="AI7" s="5">
         <v>0</v>
       </c>
       <c r="AJ7" s="5">
         <v>0</v>
       </c>
-      <c r="AK7" s="5">
-        <v>0</v>
+      <c r="AK7" s="6">
+        <v>1</v>
       </c>
       <c r="AL7" s="5">
         <v>0</v>
@@ -1926,8 +2052,8 @@
       <c r="AM7" s="5">
         <v>0</v>
       </c>
-      <c r="AN7" s="5">
-        <v>0</v>
+      <c r="AN7" s="6">
+        <v>1</v>
       </c>
       <c r="AO7" s="5">
         <v>0</v>
@@ -1947,44 +2073,44 @@
       <c r="AT7" s="5">
         <v>0</v>
       </c>
-      <c r="AU7" s="1">
-        <v>0</v>
-      </c>
-      <c r="AV7" s="5">
-        <v>0</v>
-      </c>
-      <c r="AW7" s="5">
-        <v>0</v>
+      <c r="AU7" s="5">
+        <v>0</v>
+      </c>
+      <c r="AV7" s="6">
+        <v>1</v>
+      </c>
+      <c r="AW7" s="6">
+        <v>1</v>
       </c>
       <c r="AX7" s="5">
         <v>0</v>
       </c>
-      <c r="AY7" s="5">
-        <v>0</v>
-      </c>
-      <c r="AZ7" s="6">
-        <v>1</v>
+      <c r="AY7" s="6">
+        <v>1</v>
+      </c>
+      <c r="AZ7" s="4">
+        <v>0</v>
       </c>
       <c r="BA7" s="5">
         <v>0</v>
       </c>
-      <c r="BB7" s="6">
-        <v>1</v>
+      <c r="BB7" s="5">
+        <v>0</v>
       </c>
       <c r="BC7" s="5">
         <v>0</v>
       </c>
-      <c r="BD7" s="5">
-        <v>0</v>
+      <c r="BD7" s="6">
+        <v>1</v>
       </c>
       <c r="BE7" s="5">
         <v>0</v>
       </c>
-      <c r="BF7" s="6">
-        <v>1</v>
-      </c>
-      <c r="BG7" s="6">
-        <v>1</v>
+      <c r="BF7" s="1">
+        <v>0</v>
+      </c>
+      <c r="BG7" s="5">
+        <v>0</v>
       </c>
       <c r="BH7" s="6">
         <v>1</v>
@@ -1992,8 +2118,8 @@
       <c r="BI7" s="5">
         <v>0</v>
       </c>
-      <c r="BJ7" s="5">
-        <v>0</v>
+      <c r="BJ7" s="6">
+        <v>1</v>
       </c>
       <c r="BK7" s="6">
         <v>1</v>
@@ -2003,35 +2129,35 @@
       <c r="A8" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="B8" s="6">
-        <v>1</v>
-      </c>
-      <c r="C8" s="5">
-        <v>0</v>
+      <c r="B8" s="5">
+        <v>0</v>
+      </c>
+      <c r="C8" s="6">
+        <v>1</v>
       </c>
       <c r="D8" s="6">
         <v>1</v>
       </c>
-      <c r="E8" s="5">
-        <v>0</v>
+      <c r="E8" s="6">
+        <v>1</v>
       </c>
       <c r="F8" s="5">
         <v>0</v>
       </c>
-      <c r="G8" s="6">
-        <v>1</v>
-      </c>
-      <c r="H8" s="6">
-        <v>1</v>
-      </c>
-      <c r="I8" s="6">
-        <v>1</v>
-      </c>
-      <c r="J8" s="6">
-        <v>1</v>
-      </c>
-      <c r="K8" s="6">
-        <v>1</v>
+      <c r="G8" s="5">
+        <v>0</v>
+      </c>
+      <c r="H8" s="5">
+        <v>0</v>
+      </c>
+      <c r="I8" s="5">
+        <v>0</v>
+      </c>
+      <c r="J8" s="5">
+        <v>0</v>
+      </c>
+      <c r="K8" s="5">
+        <v>0</v>
       </c>
       <c r="L8" s="5">
         <v>0</v>
@@ -2045,8 +2171,8 @@
       <c r="O8" s="5">
         <v>0</v>
       </c>
-      <c r="P8" s="6">
-        <v>1</v>
+      <c r="P8" s="5">
+        <v>0</v>
       </c>
       <c r="Q8" s="5">
         <v>0</v>
@@ -2069,17 +2195,17 @@
       <c r="W8" s="5">
         <v>0</v>
       </c>
-      <c r="X8" s="6">
-        <v>1</v>
+      <c r="X8" s="5">
+        <v>0</v>
       </c>
       <c r="Y8" s="5">
         <v>0</v>
       </c>
-      <c r="Z8" s="6">
-        <v>1</v>
-      </c>
-      <c r="AA8" s="6">
-        <v>1</v>
+      <c r="Z8" s="5">
+        <v>0</v>
+      </c>
+      <c r="AA8" s="1">
+        <v>0</v>
       </c>
       <c r="AB8" s="5">
         <v>0</v>
@@ -2102,7 +2228,7 @@
       <c r="AH8" s="5">
         <v>0</v>
       </c>
-      <c r="AI8" s="1">
+      <c r="AI8" s="5">
         <v>0</v>
       </c>
       <c r="AJ8" s="5">
@@ -2111,8 +2237,8 @@
       <c r="AK8" s="5">
         <v>0</v>
       </c>
-      <c r="AL8" s="6">
-        <v>1</v>
+      <c r="AL8" s="5">
+        <v>0</v>
       </c>
       <c r="AM8" s="5">
         <v>0</v>
@@ -2126,11 +2252,11 @@
       <c r="AP8" s="5">
         <v>0</v>
       </c>
-      <c r="AQ8" s="5">
-        <v>0</v>
-      </c>
-      <c r="AR8" s="6">
-        <v>1</v>
+      <c r="AQ8" s="6">
+        <v>1</v>
+      </c>
+      <c r="AR8" s="5">
+        <v>0</v>
       </c>
       <c r="AS8" s="5">
         <v>0</v>
@@ -2138,7 +2264,7 @@
       <c r="AT8" s="5">
         <v>0</v>
       </c>
-      <c r="AU8" s="1">
+      <c r="AU8" s="5">
         <v>0</v>
       </c>
       <c r="AV8" s="5">
@@ -2153,48 +2279,48 @@
       <c r="AY8" s="5">
         <v>0</v>
       </c>
-      <c r="AZ8" s="5">
-        <v>0</v>
-      </c>
-      <c r="BA8" s="5">
-        <v>0</v>
-      </c>
-      <c r="BB8" s="5">
-        <v>0</v>
-      </c>
-      <c r="BC8" s="5">
-        <v>0</v>
+      <c r="AZ8" s="6">
+        <v>1</v>
+      </c>
+      <c r="BA8" s="6">
+        <v>1</v>
+      </c>
+      <c r="BB8" s="6">
+        <v>1</v>
+      </c>
+      <c r="BC8" s="6">
+        <v>1</v>
       </c>
       <c r="BD8" s="5">
         <v>0</v>
       </c>
-      <c r="BE8" s="5">
-        <v>0</v>
-      </c>
-      <c r="BF8" s="5">
+      <c r="BE8" s="6">
+        <v>1</v>
+      </c>
+      <c r="BF8" s="1">
         <v>0</v>
       </c>
       <c r="BG8" s="5">
         <v>0</v>
       </c>
-      <c r="BH8" s="5">
-        <v>0</v>
-      </c>
-      <c r="BI8" s="5">
-        <v>0</v>
-      </c>
-      <c r="BJ8" s="5">
-        <v>0</v>
-      </c>
-      <c r="BK8" s="5">
-        <v>0</v>
+      <c r="BH8" s="6">
+        <v>1</v>
+      </c>
+      <c r="BI8" s="6">
+        <v>1</v>
+      </c>
+      <c r="BJ8" s="6">
+        <v>1</v>
+      </c>
+      <c r="BK8" s="6">
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:63" s="4" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="B9" s="6">
+      <c r="B9" s="5">
         <v>1</v>
       </c>
       <c r="C9" s="5">
@@ -2203,17 +2329,17 @@
       <c r="D9" s="5">
         <v>0</v>
       </c>
-      <c r="E9" s="6">
-        <v>1</v>
+      <c r="E9" s="5">
+        <v>0</v>
       </c>
       <c r="F9" s="5">
-        <v>1</v>
-      </c>
-      <c r="G9" s="6">
-        <v>1</v>
-      </c>
-      <c r="H9" s="6">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="G9" s="5">
+        <v>0</v>
+      </c>
+      <c r="H9" s="5">
+        <v>0</v>
       </c>
       <c r="I9" s="5">
         <v>0</v>
@@ -2236,8 +2362,8 @@
       <c r="O9" s="5">
         <v>0</v>
       </c>
-      <c r="P9" s="6">
-        <v>1</v>
+      <c r="P9" s="5">
+        <v>0</v>
       </c>
       <c r="Q9" s="5">
         <v>0</v>
@@ -2245,8 +2371,8 @@
       <c r="R9" s="5">
         <v>0</v>
       </c>
-      <c r="S9" s="6">
-        <v>1</v>
+      <c r="S9" s="5">
+        <v>0</v>
       </c>
       <c r="T9" s="5">
         <v>0</v>
@@ -2260,17 +2386,17 @@
       <c r="W9" s="5">
         <v>0</v>
       </c>
-      <c r="X9" s="6">
-        <v>1</v>
+      <c r="X9" s="5">
+        <v>0</v>
       </c>
       <c r="Y9" s="5">
         <v>0</v>
       </c>
-      <c r="Z9" s="6">
-        <v>1</v>
-      </c>
-      <c r="AA9" s="6">
-        <v>1</v>
+      <c r="Z9" s="5">
+        <v>0</v>
+      </c>
+      <c r="AA9" s="1">
+        <v>0</v>
       </c>
       <c r="AB9" s="5">
         <v>0</v>
@@ -2293,8 +2419,8 @@
       <c r="AH9" s="5">
         <v>0</v>
       </c>
-      <c r="AI9" s="1">
-        <v>1</v>
+      <c r="AI9" s="5">
+        <v>0</v>
       </c>
       <c r="AJ9" s="5">
         <v>0</v>
@@ -2302,8 +2428,8 @@
       <c r="AK9" s="5">
         <v>0</v>
       </c>
-      <c r="AL9" s="6">
-        <v>1</v>
+      <c r="AL9" s="5">
+        <v>0</v>
       </c>
       <c r="AM9" s="5">
         <v>0</v>
@@ -2320,8 +2446,8 @@
       <c r="AQ9" s="5">
         <v>0</v>
       </c>
-      <c r="AR9" s="6">
-        <v>1</v>
+      <c r="AR9" s="5">
+        <v>0</v>
       </c>
       <c r="AS9" s="5">
         <v>0</v>
@@ -2329,7 +2455,7 @@
       <c r="AT9" s="5">
         <v>0</v>
       </c>
-      <c r="AU9" s="1">
+      <c r="AU9" s="5">
         <v>0</v>
       </c>
       <c r="AV9" s="5">
@@ -2338,47 +2464,47 @@
       <c r="AW9" s="5">
         <v>0</v>
       </c>
-      <c r="AX9" s="5">
-        <v>0</v>
+      <c r="AX9" s="6">
+        <v>1</v>
       </c>
       <c r="AY9" s="5">
         <v>0</v>
       </c>
-      <c r="AZ9" s="5">
-        <v>0</v>
-      </c>
-      <c r="BA9" s="5">
-        <v>0</v>
-      </c>
-      <c r="BB9" s="5">
-        <v>0</v>
-      </c>
-      <c r="BC9" s="5">
-        <v>0</v>
+      <c r="AZ9" s="6">
+        <v>1</v>
+      </c>
+      <c r="BA9" s="6">
+        <v>1</v>
+      </c>
+      <c r="BB9" s="6">
+        <v>1</v>
+      </c>
+      <c r="BC9" s="6">
+        <v>1</v>
       </c>
       <c r="BD9" s="5">
         <v>0</v>
       </c>
-      <c r="BE9" s="5">
-        <v>0</v>
-      </c>
-      <c r="BF9" s="5">
-        <v>0</v>
-      </c>
-      <c r="BG9" s="5">
-        <v>0</v>
-      </c>
-      <c r="BH9" s="5">
-        <v>0</v>
-      </c>
-      <c r="BI9" s="5">
-        <v>0</v>
-      </c>
-      <c r="BJ9" s="5">
-        <v>0</v>
-      </c>
-      <c r="BK9" s="5">
-        <v>0</v>
+      <c r="BE9" s="6">
+        <v>1</v>
+      </c>
+      <c r="BF9" s="1">
+        <v>1</v>
+      </c>
+      <c r="BG9" s="6">
+        <v>1</v>
+      </c>
+      <c r="BH9" s="6">
+        <v>1</v>
+      </c>
+      <c r="BI9" s="6">
+        <v>1</v>
+      </c>
+      <c r="BJ9" s="6">
+        <v>1</v>
+      </c>
+      <c r="BK9" s="6">
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:63" s="4" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -2394,17 +2520,17 @@
       <c r="D10" s="5">
         <v>0</v>
       </c>
-      <c r="E10" s="6">
-        <v>1</v>
+      <c r="E10" s="5">
+        <v>0</v>
       </c>
       <c r="F10" s="5">
         <v>0</v>
       </c>
-      <c r="G10" s="6">
-        <v>1</v>
-      </c>
-      <c r="H10" s="6">
-        <v>1</v>
+      <c r="G10" s="5">
+        <v>0</v>
+      </c>
+      <c r="H10" s="5">
+        <v>0</v>
       </c>
       <c r="I10" s="5">
         <v>0</v>
@@ -2421,26 +2547,26 @@
       <c r="M10" s="5">
         <v>0</v>
       </c>
-      <c r="N10" s="5">
-        <v>0</v>
+      <c r="N10" s="6">
+        <v>1</v>
       </c>
       <c r="O10" s="5">
         <v>0</v>
       </c>
-      <c r="P10" s="6">
-        <v>1</v>
+      <c r="P10" s="5">
+        <v>0</v>
       </c>
       <c r="Q10" s="5">
         <v>0</v>
       </c>
-      <c r="R10" s="6">
-        <v>1</v>
+      <c r="R10" s="5">
+        <v>0</v>
       </c>
       <c r="S10" s="5">
         <v>0</v>
       </c>
-      <c r="T10" s="6">
-        <v>1</v>
+      <c r="T10" s="5">
+        <v>0</v>
       </c>
       <c r="U10" s="5">
         <v>0</v>
@@ -2460,17 +2586,17 @@
       <c r="Z10" s="5">
         <v>0</v>
       </c>
-      <c r="AA10" s="6">
-        <v>1</v>
-      </c>
-      <c r="AB10" s="6">
-        <v>1</v>
-      </c>
-      <c r="AC10" s="6">
-        <v>1</v>
-      </c>
-      <c r="AD10" s="5">
-        <v>0</v>
+      <c r="AA10" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB10" s="5">
+        <v>0</v>
+      </c>
+      <c r="AC10" s="5">
+        <v>0</v>
+      </c>
+      <c r="AD10" s="6">
+        <v>1</v>
       </c>
       <c r="AE10" s="5">
         <v>0</v>
@@ -2481,11 +2607,11 @@
       <c r="AG10" s="5">
         <v>0</v>
       </c>
-      <c r="AH10" s="5">
-        <v>0</v>
-      </c>
-      <c r="AI10" s="1">
-        <v>1</v>
+      <c r="AH10" s="6">
+        <v>1</v>
+      </c>
+      <c r="AI10" s="5">
+        <v>0</v>
       </c>
       <c r="AJ10" s="5">
         <v>0</v>
@@ -2493,17 +2619,17 @@
       <c r="AK10" s="5">
         <v>0</v>
       </c>
-      <c r="AL10" s="5">
-        <v>0</v>
-      </c>
-      <c r="AM10" s="6">
-        <v>1</v>
+      <c r="AL10" s="6">
+        <v>1</v>
+      </c>
+      <c r="AM10" s="5">
+        <v>0</v>
       </c>
       <c r="AN10" s="5">
         <v>0</v>
       </c>
-      <c r="AO10" s="5">
-        <v>0</v>
+      <c r="AO10" s="6">
+        <v>1</v>
       </c>
       <c r="AP10" s="5">
         <v>0</v>
@@ -2511,29 +2637,29 @@
       <c r="AQ10" s="5">
         <v>0</v>
       </c>
-      <c r="AR10" s="6">
-        <v>1</v>
+      <c r="AR10" s="5">
+        <v>0</v>
       </c>
       <c r="AS10" s="5">
         <v>0</v>
       </c>
-      <c r="AT10" s="5">
-        <v>0</v>
-      </c>
-      <c r="AU10" s="1">
-        <v>0</v>
-      </c>
-      <c r="AV10" s="5">
-        <v>0</v>
-      </c>
-      <c r="AW10" s="5">
-        <v>0</v>
-      </c>
-      <c r="AX10" s="6">
-        <v>1</v>
-      </c>
-      <c r="AY10" s="5">
-        <v>0</v>
+      <c r="AT10" s="6">
+        <v>1</v>
+      </c>
+      <c r="AU10" s="5">
+        <v>0</v>
+      </c>
+      <c r="AV10" s="6">
+        <v>1</v>
+      </c>
+      <c r="AW10" s="6">
+        <v>1</v>
+      </c>
+      <c r="AX10" s="5">
+        <v>0</v>
+      </c>
+      <c r="AY10" s="6">
+        <v>1</v>
       </c>
       <c r="AZ10" s="5">
         <v>0</v>
@@ -2547,29 +2673,29 @@
       <c r="BC10" s="6">
         <v>1</v>
       </c>
-      <c r="BD10" s="5">
-        <v>0</v>
-      </c>
-      <c r="BE10" s="5">
-        <v>0</v>
-      </c>
-      <c r="BF10" s="6">
-        <v>1</v>
-      </c>
-      <c r="BG10" s="5">
-        <v>0</v>
+      <c r="BD10" s="6">
+        <v>1</v>
+      </c>
+      <c r="BE10" s="6">
+        <v>1</v>
+      </c>
+      <c r="BF10" s="1">
+        <v>1</v>
+      </c>
+      <c r="BG10" s="6">
+        <v>1</v>
       </c>
       <c r="BH10" s="6">
         <v>1</v>
       </c>
-      <c r="BI10" s="6">
-        <v>1</v>
-      </c>
-      <c r="BJ10" s="5">
-        <v>0</v>
-      </c>
-      <c r="BK10" s="5">
-        <v>0</v>
+      <c r="BI10" s="5">
+        <v>0</v>
+      </c>
+      <c r="BJ10" s="6">
+        <v>1</v>
+      </c>
+      <c r="BK10" s="6">
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:63" s="4" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -2579,8 +2705,8 @@
       <c r="B11" s="5">
         <v>0</v>
       </c>
-      <c r="C11" s="6">
-        <v>1</v>
+      <c r="C11" s="5">
+        <v>0</v>
       </c>
       <c r="D11" s="5">
         <v>0</v>
@@ -2594,11 +2720,11 @@
       <c r="G11" s="5">
         <v>0</v>
       </c>
-      <c r="H11" s="6">
-        <v>1</v>
-      </c>
-      <c r="I11" s="5">
-        <v>0</v>
+      <c r="H11" s="5">
+        <v>0</v>
+      </c>
+      <c r="I11" s="6">
+        <v>1</v>
       </c>
       <c r="J11" s="5">
         <v>0</v>
@@ -2609,17 +2735,17 @@
       <c r="L11" s="5">
         <v>0</v>
       </c>
-      <c r="M11" s="5">
-        <v>0</v>
+      <c r="M11" s="6">
+        <v>1</v>
       </c>
       <c r="N11" s="5">
         <v>0</v>
       </c>
-      <c r="O11" s="6">
-        <v>1</v>
-      </c>
-      <c r="P11" s="6">
-        <v>1</v>
+      <c r="O11" s="5">
+        <v>0</v>
+      </c>
+      <c r="P11" s="5">
+        <v>0</v>
       </c>
       <c r="Q11" s="5">
         <v>0</v>
@@ -2627,17 +2753,17 @@
       <c r="R11" s="5">
         <v>0</v>
       </c>
-      <c r="S11" s="6">
-        <v>1</v>
-      </c>
-      <c r="T11" s="6">
-        <v>1</v>
+      <c r="S11" s="5">
+        <v>0</v>
+      </c>
+      <c r="T11" s="5">
+        <v>0</v>
       </c>
       <c r="U11" s="5">
         <v>0</v>
       </c>
-      <c r="V11" s="6">
-        <v>1</v>
+      <c r="V11" s="5">
+        <v>0</v>
       </c>
       <c r="W11" s="5">
         <v>0</v>
@@ -2645,17 +2771,17 @@
       <c r="X11" s="5">
         <v>0</v>
       </c>
-      <c r="Y11" s="6">
-        <v>1</v>
+      <c r="Y11" s="5">
+        <v>0</v>
       </c>
       <c r="Z11" s="5">
         <v>0</v>
       </c>
-      <c r="AA11" s="5">
-        <v>0</v>
-      </c>
-      <c r="AB11" s="6">
-        <v>1</v>
+      <c r="AA11" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB11" s="5">
+        <v>0</v>
       </c>
       <c r="AC11" s="5">
         <v>0</v>
@@ -2663,8 +2789,8 @@
       <c r="AD11" s="5">
         <v>0</v>
       </c>
-      <c r="AE11" s="5">
-        <v>0</v>
+      <c r="AE11" s="6">
+        <v>1</v>
       </c>
       <c r="AF11" s="5">
         <v>0</v>
@@ -2672,10 +2798,10 @@
       <c r="AG11" s="5">
         <v>0</v>
       </c>
-      <c r="AH11" s="6">
-        <v>1</v>
-      </c>
-      <c r="AI11" s="1">
+      <c r="AH11" s="5">
+        <v>0</v>
+      </c>
+      <c r="AI11" s="5">
         <v>0</v>
       </c>
       <c r="AJ11" s="5">
@@ -2684,11 +2810,11 @@
       <c r="AK11" s="5">
         <v>0</v>
       </c>
-      <c r="AL11" s="6">
-        <v>1</v>
-      </c>
-      <c r="AM11" s="6">
-        <v>1</v>
+      <c r="AL11" s="5">
+        <v>0</v>
+      </c>
+      <c r="AM11" s="5">
+        <v>0</v>
       </c>
       <c r="AN11" s="5">
         <v>0</v>
@@ -2696,22 +2822,22 @@
       <c r="AO11" s="5">
         <v>0</v>
       </c>
-      <c r="AP11" s="5">
-        <v>0</v>
+      <c r="AP11" s="6">
+        <v>1</v>
       </c>
       <c r="AQ11" s="5">
         <v>0</v>
       </c>
-      <c r="AR11" s="5">
-        <v>0</v>
-      </c>
-      <c r="AS11" s="5">
-        <v>0</v>
-      </c>
-      <c r="AT11" s="5">
-        <v>0</v>
-      </c>
-      <c r="AU11" s="1">
+      <c r="AR11" s="6">
+        <v>1</v>
+      </c>
+      <c r="AS11" s="6">
+        <v>1</v>
+      </c>
+      <c r="AT11" s="6">
+        <v>1</v>
+      </c>
+      <c r="AU11" s="5">
         <v>0</v>
       </c>
       <c r="AV11" s="5">
@@ -2720,8 +2846,8 @@
       <c r="AW11" s="5">
         <v>0</v>
       </c>
-      <c r="AX11" s="5">
-        <v>0</v>
+      <c r="AX11" s="6">
+        <v>1</v>
       </c>
       <c r="AY11" s="6">
         <v>1</v>
@@ -2738,279 +2864,655 @@
       <c r="BC11" s="5">
         <v>0</v>
       </c>
-      <c r="BD11" s="5">
-        <v>0</v>
+      <c r="BD11" s="6">
+        <v>1</v>
       </c>
       <c r="BE11" s="5">
         <v>0</v>
       </c>
-      <c r="BF11" s="5">
+      <c r="BF11" s="1">
         <v>0</v>
       </c>
       <c r="BG11" s="5">
         <v>0</v>
       </c>
-      <c r="BH11" s="5">
-        <v>0</v>
-      </c>
-      <c r="BI11" s="5">
-        <v>0</v>
+      <c r="BH11" s="6">
+        <v>1</v>
+      </c>
+      <c r="BI11" s="6">
+        <v>1</v>
       </c>
       <c r="BJ11" s="5">
         <v>0</v>
       </c>
-      <c r="BK11" s="5">
-        <v>0</v>
+      <c r="BK11" s="6">
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:63" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="1">
+      <c r="B13" s="2">
         <f>SUM(B2:B11)</f>
+        <v>1</v>
+      </c>
+      <c r="C13" s="2">
+        <f>SUM(C2:C11)</f>
+        <v>1</v>
+      </c>
+      <c r="D13" s="2">
+        <f>SUM(D2:D11)</f>
+        <v>1</v>
+      </c>
+      <c r="E13" s="2">
+        <f>SUM(E2:E11)</f>
+        <v>1</v>
+      </c>
+      <c r="F13" s="2">
+        <f>SUM(F2:F11)</f>
+        <v>1</v>
+      </c>
+      <c r="G13" s="2">
+        <f>SUM(G2:G11)</f>
+        <v>1</v>
+      </c>
+      <c r="H13" s="2">
+        <f>SUM(H2:H11)</f>
+        <v>1</v>
+      </c>
+      <c r="I13" s="2">
+        <f>SUM(I2:I11)</f>
+        <v>1</v>
+      </c>
+      <c r="J13" s="2">
+        <f>SUM(J2:J11)</f>
+        <v>1</v>
+      </c>
+      <c r="K13" s="2">
+        <f>SUM(K2:K11)</f>
+        <v>1</v>
+      </c>
+      <c r="L13" s="2">
+        <f>SUM(L2:L11)</f>
+        <v>1</v>
+      </c>
+      <c r="M13" s="2">
+        <f>SUM(M2:M11)</f>
+        <v>1</v>
+      </c>
+      <c r="N13" s="2">
+        <f>SUM(N2:N11)</f>
+        <v>1</v>
+      </c>
+      <c r="O13" s="2">
+        <f>SUM(O2:O11)</f>
+        <v>1</v>
+      </c>
+      <c r="P13" s="2">
+        <f>SUM(P2:P11)</f>
+        <v>1</v>
+      </c>
+      <c r="Q13" s="2">
+        <f>SUM(Q2:Q11)</f>
+        <v>1</v>
+      </c>
+      <c r="R13" s="2">
+        <f>SUM(R2:R11)</f>
+        <v>1</v>
+      </c>
+      <c r="S13" s="2">
+        <f>SUM(S2:S11)</f>
+        <v>1</v>
+      </c>
+      <c r="T13" s="2">
+        <f>SUM(T2:T11)</f>
+        <v>1</v>
+      </c>
+      <c r="U13" s="2">
+        <f>SUM(U2:U11)</f>
+        <v>1</v>
+      </c>
+      <c r="V13" s="2">
+        <f>SUM(V2:V11)</f>
+        <v>1</v>
+      </c>
+      <c r="W13" s="2">
+        <f>SUM(W2:W11)</f>
+        <v>1</v>
+      </c>
+      <c r="X13" s="2">
+        <f>SUM(X2:X11)</f>
+        <v>1</v>
+      </c>
+      <c r="Y13" s="2">
+        <f>SUM(Y2:Y11)</f>
+        <v>1</v>
+      </c>
+      <c r="Z13" s="2">
+        <f>SUM(Z2:Z11)</f>
+        <v>1</v>
+      </c>
+      <c r="AA13" s="2">
+        <f>SUM(AA2:AA11)</f>
+        <v>1</v>
+      </c>
+      <c r="AB13" s="2">
+        <f>SUM(AB2:AB11)</f>
+        <v>1</v>
+      </c>
+      <c r="AC13" s="2">
+        <f>SUM(AC2:AC11)</f>
+        <v>1</v>
+      </c>
+      <c r="AD13" s="2">
+        <f>SUM(AD2:AD11)</f>
+        <v>1</v>
+      </c>
+      <c r="AE13" s="2">
+        <f>SUM(AE2:AE11)</f>
+        <v>1</v>
+      </c>
+      <c r="AF13" s="2">
+        <f>SUM(AF2:AF11)</f>
+        <v>1</v>
+      </c>
+      <c r="AG13" s="2">
+        <f>SUM(AG2:AG11)</f>
+        <v>1</v>
+      </c>
+      <c r="AH13" s="2">
+        <f>SUM(AH2:AH11)</f>
+        <v>1</v>
+      </c>
+      <c r="AI13" s="2">
+        <f>SUM(AI2:AI11)</f>
+        <v>1</v>
+      </c>
+      <c r="AJ13" s="2">
+        <f>SUM(AJ2:AJ11)</f>
+        <v>1</v>
+      </c>
+      <c r="AK13" s="2">
+        <f>SUM(AK2:AK11)</f>
+        <v>1</v>
+      </c>
+      <c r="AL13" s="2">
+        <f>SUM(AL2:AL11)</f>
+        <v>1</v>
+      </c>
+      <c r="AM13" s="2">
+        <f>SUM(AM2:AM11)</f>
+        <v>1</v>
+      </c>
+      <c r="AN13" s="2">
+        <f>SUM(AN2:AN11)</f>
+        <v>1</v>
+      </c>
+      <c r="AO13" s="2">
+        <f>SUM(AO2:AO11)</f>
+        <v>2</v>
+      </c>
+      <c r="AP13" s="2">
+        <f>SUM(AP2:AP11)</f>
+        <v>2</v>
+      </c>
+      <c r="AQ13" s="2">
+        <f>SUM(AQ2:AQ11)</f>
+        <v>2</v>
+      </c>
+      <c r="AR13" s="2">
+        <f>SUM(AR2:AR11)</f>
+        <v>2</v>
+      </c>
+      <c r="AS13" s="2">
+        <f>SUM(AS2:AS11)</f>
+        <v>2</v>
+      </c>
+      <c r="AT13" s="2">
+        <f>SUM(AT2:AT11)</f>
+        <v>2</v>
+      </c>
+      <c r="AU13" s="2">
+        <f>SUM(AU2:AU11)</f>
+        <v>2</v>
+      </c>
+      <c r="AV13" s="2">
+        <f>SUM(AV2:AV11)</f>
+        <v>2</v>
+      </c>
+      <c r="AW13" s="2">
+        <f>SUM(AW2:AW11)</f>
+        <v>2</v>
+      </c>
+      <c r="AX13" s="2">
+        <f>SUM(AX2:AX11)</f>
         <v>3</v>
       </c>
-      <c r="C13" s="1">
-        <f t="shared" ref="C13:BK13" si="0">SUM(C2:C11)</f>
+      <c r="AY13" s="2">
+        <f>SUM(AY2:AY11)</f>
+        <v>3</v>
+      </c>
+      <c r="AZ13" s="2">
+        <f>SUM(AZ2:AZ11)</f>
+        <v>3</v>
+      </c>
+      <c r="BA13" s="2">
+        <f>SUM(BA2:BA11)</f>
+        <v>3</v>
+      </c>
+      <c r="BB13" s="2">
+        <f>SUM(BB2:BB11)</f>
+        <v>3</v>
+      </c>
+      <c r="BC13" s="2">
+        <f>SUM(BC2:BC11)</f>
+        <v>3</v>
+      </c>
+      <c r="BD13" s="2">
+        <f>SUM(BD2:BD11)</f>
+        <v>3</v>
+      </c>
+      <c r="BE13" s="2">
+        <f>SUM(BE2:BE11)</f>
+        <v>3</v>
+      </c>
+      <c r="BF13" s="2">
+        <f>SUM(BF2:BF11)</f>
+        <v>4</v>
+      </c>
+      <c r="BG13" s="2">
+        <f>SUM(BG2:BG11)</f>
+        <v>4</v>
+      </c>
+      <c r="BH13" s="2">
+        <f>SUM(BH2:BH11)</f>
+        <v>5</v>
+      </c>
+      <c r="BI13" s="2">
+        <f>SUM(BI2:BI11)</f>
+        <v>5</v>
+      </c>
+      <c r="BJ13" s="2">
+        <f>SUM(BJ2:BJ11)</f>
+        <v>6</v>
+      </c>
+      <c r="BK13" s="2">
+        <f>SUM(BK2:BK11)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:63" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B15" s="1">
+        <v>124</v>
+      </c>
+      <c r="C15" s="1">
+        <v>122</v>
+      </c>
+      <c r="D15" s="1">
+        <v>120</v>
+      </c>
+      <c r="E15" s="1">
+        <v>118</v>
+      </c>
+      <c r="F15" s="1">
+        <v>116</v>
+      </c>
+      <c r="G15" s="1">
+        <v>114</v>
+      </c>
+      <c r="H15" s="1">
+        <v>112</v>
+      </c>
+      <c r="I15" s="1">
+        <v>110</v>
+      </c>
+      <c r="J15" s="1">
+        <v>108</v>
+      </c>
+      <c r="K15" s="1">
+        <v>106</v>
+      </c>
+      <c r="L15" s="1">
+        <v>104</v>
+      </c>
+      <c r="M15" s="1">
+        <v>102</v>
+      </c>
+      <c r="N15" s="1">
+        <v>100</v>
+      </c>
+      <c r="O15" s="1">
+        <v>98</v>
+      </c>
+      <c r="P15" s="1">
+        <v>96</v>
+      </c>
+      <c r="Q15" s="1">
+        <v>94</v>
+      </c>
+      <c r="R15" s="1">
+        <v>92</v>
+      </c>
+      <c r="S15" s="1">
+        <v>90</v>
+      </c>
+      <c r="T15" s="1">
+        <v>88</v>
+      </c>
+      <c r="U15" s="1">
+        <v>86</v>
+      </c>
+      <c r="V15" s="1">
+        <v>84</v>
+      </c>
+      <c r="W15" s="1">
+        <v>82</v>
+      </c>
+      <c r="X15" s="1">
+        <v>80</v>
+      </c>
+      <c r="Y15" s="1">
+        <v>78</v>
+      </c>
+      <c r="Z15" s="1">
+        <v>76</v>
+      </c>
+      <c r="AA15" s="1">
+        <v>74</v>
+      </c>
+      <c r="AB15" s="1">
+        <v>72</v>
+      </c>
+      <c r="AC15" s="1">
+        <v>70</v>
+      </c>
+      <c r="AD15" s="1">
+        <v>68</v>
+      </c>
+      <c r="AE15" s="1">
+        <v>66</v>
+      </c>
+      <c r="AF15" s="1">
+        <v>64</v>
+      </c>
+      <c r="AG15" s="1">
+        <v>62</v>
+      </c>
+      <c r="AH15" s="1">
+        <v>60</v>
+      </c>
+      <c r="AI15" s="1">
+        <v>58</v>
+      </c>
+      <c r="AJ15" s="1">
+        <v>56</v>
+      </c>
+      <c r="AK15" s="1">
+        <v>54</v>
+      </c>
+      <c r="AL15" s="1">
+        <v>52</v>
+      </c>
+      <c r="AM15" s="1">
+        <v>50</v>
+      </c>
+      <c r="AN15" s="1">
+        <v>48</v>
+      </c>
+      <c r="AO15" s="1">
+        <v>46</v>
+      </c>
+      <c r="AP15" s="1">
+        <v>44</v>
+      </c>
+      <c r="AQ15" s="1">
+        <v>42</v>
+      </c>
+      <c r="AR15" s="1">
+        <v>40</v>
+      </c>
+      <c r="AS15" s="1">
+        <v>38</v>
+      </c>
+      <c r="AT15" s="1">
+        <v>36</v>
+      </c>
+      <c r="AU15" s="1">
+        <v>34</v>
+      </c>
+      <c r="AV15" s="1">
+        <v>32</v>
+      </c>
+      <c r="AW15" s="1">
+        <v>30</v>
+      </c>
+      <c r="AX15" s="1">
+        <v>28</v>
+      </c>
+      <c r="AY15" s="1">
+        <v>26</v>
+      </c>
+      <c r="AZ15" s="1">
+        <v>24</v>
+      </c>
+      <c r="BA15" s="1">
+        <v>22</v>
+      </c>
+      <c r="BB15" s="1">
+        <v>20</v>
+      </c>
+      <c r="BC15" s="1">
+        <v>18</v>
+      </c>
+      <c r="BD15" s="1">
+        <v>16</v>
+      </c>
+      <c r="BE15" s="1">
+        <v>14</v>
+      </c>
+      <c r="BF15" s="1">
+        <v>12</v>
+      </c>
+      <c r="BG15" s="1">
+        <v>10</v>
+      </c>
+      <c r="BH15" s="1">
+        <v>8</v>
+      </c>
+      <c r="BI15" s="1">
+        <v>6</v>
+      </c>
+      <c r="BJ15" s="1">
+        <v>4</v>
+      </c>
+      <c r="BK15" s="1">
         <v>2</v>
       </c>
-      <c r="D13" s="1">
-        <f t="shared" si="0"/>
+    </row>
+    <row r="16" spans="1:63" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B16" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M16" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N16" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="O16" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="P16" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q16" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="R16" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="S16" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="T16" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="U16" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="V16" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="W16" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="X16" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y16" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z16" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AA16" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="AB16" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AC16" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AD16" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AE16" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AF16" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AG16" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AH16" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AI16" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="AJ16" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AK16" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AL16" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AM16" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AN16" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AO16" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="AP16" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AQ16" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E13" s="1">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="F13" s="1">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="G13" s="1">
-        <f t="shared" si="0"/>
+      <c r="AR16" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="AS16" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AT16" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AU16" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AV16" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AW16" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AX16" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AY16" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="AZ16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="BA16" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="BB16" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="BC16" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="BD16" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="BE16" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="BF16" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="BG16" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="BH16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="BI16" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="BJ16" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="BK16" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="H13" s="1">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="I13" s="1">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="J13" s="1">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="K13" s="1">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="L13" s="1">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="M13" s="1">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="N13" s="1">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="O13" s="1">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="P13" s="1">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="Q13" s="1">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="R13" s="1">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="S13" s="1">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="T13" s="1">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="U13" s="1">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="V13" s="1">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="W13" s="1">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="X13" s="1">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="Y13" s="1">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="Z13" s="1">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="AA13" s="1">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="AB13" s="1">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="AC13" s="1">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="AD13" s="1">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="AE13" s="1">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="AF13" s="1">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="AG13" s="1">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="AH13" s="1">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="AI13" s="1">
-        <f>SUM(AI2:AI11)</f>
-        <v>4</v>
-      </c>
-      <c r="AJ13" s="1">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="AK13" s="1">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="AL13" s="1">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="AM13" s="1">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="AN13" s="1">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="AO13" s="1">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="AP13" s="1">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="AQ13" s="1">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="AR13" s="1">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="AS13" s="1">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="AT13" s="1">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="AU13" s="1">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="AV13" s="1">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="AW13" s="1">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="AX13" s="1">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="AY13" s="1">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="AZ13" s="1">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="BA13" s="1">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="BB13" s="1">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="BC13" s="1">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="BD13" s="1">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="BE13" s="1">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="BF13" s="1">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="BG13" s="1">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="BH13" s="1">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="BI13" s="1">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="BJ13" s="1">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="BK13" s="1">
-        <f t="shared" si="0"/>
-        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>